<commit_message>
Actualizacao da 6 sessao AG Ribaue e Monapo Reposicao
</commit_message>
<xml_diff>
--- a/Data/indiv_AG.xlsx
+++ b/Data/indiv_AG.xlsx
@@ -10723,7 +10723,7 @@
       </c>
       <c r="J155" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K155" t="inlineStr">
@@ -10790,7 +10790,7 @@
       </c>
       <c r="J156" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K156" t="inlineStr">
@@ -10857,7 +10857,7 @@
       </c>
       <c r="J157" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K157" t="inlineStr">
@@ -10924,7 +10924,7 @@
       </c>
       <c r="J158" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K158" t="inlineStr">
@@ -10986,12 +10986,12 @@
       </c>
       <c r="I159" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J159" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K159" t="inlineStr">
@@ -11053,12 +11053,12 @@
       </c>
       <c r="I160" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J160" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K160" t="inlineStr">
@@ -11120,12 +11120,12 @@
       </c>
       <c r="I161" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J161" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K161" t="inlineStr">
@@ -11254,12 +11254,12 @@
       </c>
       <c r="I163" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J163" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K163" t="inlineStr">
@@ -11326,7 +11326,7 @@
       </c>
       <c r="J164" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K164" t="inlineStr">
@@ -11388,12 +11388,12 @@
       </c>
       <c r="I165" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J165" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K165" t="inlineStr">
@@ -11527,7 +11527,7 @@
       </c>
       <c r="J167" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K167" t="inlineStr">
@@ -11594,7 +11594,7 @@
       </c>
       <c r="J168" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K168" t="inlineStr">
@@ -11656,12 +11656,12 @@
       </c>
       <c r="I169" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J169" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K169" t="inlineStr">
@@ -11723,12 +11723,12 @@
       </c>
       <c r="I170" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J170" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K170" t="inlineStr">
@@ -11790,12 +11790,12 @@
       </c>
       <c r="I171" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J171" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K171" t="inlineStr">
@@ -11862,7 +11862,7 @@
       </c>
       <c r="J172" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K172" t="inlineStr">
@@ -12063,7 +12063,7 @@
       </c>
       <c r="J175" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K175" t="inlineStr">
@@ -12125,12 +12125,12 @@
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J176" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K176" t="inlineStr">
@@ -12259,12 +12259,12 @@
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J178" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K178" t="inlineStr">
@@ -12326,12 +12326,12 @@
       </c>
       <c r="I179" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J179" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K179" t="inlineStr">
@@ -12398,7 +12398,7 @@
       </c>
       <c r="J180" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K180" t="inlineStr">
@@ -12460,12 +12460,12 @@
       </c>
       <c r="I181" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J181" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K181" t="inlineStr">
@@ -12594,12 +12594,12 @@
       </c>
       <c r="I183" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J183" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K183" t="inlineStr">
@@ -12661,12 +12661,12 @@
       </c>
       <c r="I184" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J184" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K184" t="inlineStr">
@@ -12733,7 +12733,7 @@
       </c>
       <c r="J185" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K185" t="inlineStr">
@@ -12795,12 +12795,12 @@
       </c>
       <c r="I186" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J186" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K186" t="inlineStr">
@@ -12867,7 +12867,7 @@
       </c>
       <c r="J187" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K187" t="inlineStr">
@@ -12929,12 +12929,12 @@
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J188" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K188" t="inlineStr">
@@ -13001,7 +13001,7 @@
       </c>
       <c r="J189" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K189" t="inlineStr">
@@ -13068,7 +13068,7 @@
       </c>
       <c r="J190" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K190" t="inlineStr">
@@ -13135,7 +13135,7 @@
       </c>
       <c r="J191" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K191" t="inlineStr">
@@ -13202,7 +13202,7 @@
       </c>
       <c r="J192" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K192" t="inlineStr">
@@ -13264,12 +13264,12 @@
       </c>
       <c r="I193" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J193" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K193" t="inlineStr">
@@ -13331,12 +13331,12 @@
       </c>
       <c r="I194" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J194" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K194" t="inlineStr">
@@ -13398,12 +13398,12 @@
       </c>
       <c r="I195" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J195" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K195" t="inlineStr">
@@ -13465,12 +13465,12 @@
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J196" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K196" t="inlineStr">
@@ -13537,7 +13537,7 @@
       </c>
       <c r="J197" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K197" t="inlineStr">
@@ -13604,7 +13604,7 @@
       </c>
       <c r="J198" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K198" t="inlineStr">
@@ -13671,7 +13671,7 @@
       </c>
       <c r="J199" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K199" t="inlineStr">
@@ -13738,7 +13738,7 @@
       </c>
       <c r="J200" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K200" t="inlineStr">
@@ -13805,7 +13805,7 @@
       </c>
       <c r="J201" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K201" t="inlineStr">
@@ -13872,7 +13872,7 @@
       </c>
       <c r="J202" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K202" t="inlineStr">
@@ -13939,7 +13939,7 @@
       </c>
       <c r="J203" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K203" t="inlineStr">
@@ -14006,7 +14006,7 @@
       </c>
       <c r="J204" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K204" t="inlineStr">
@@ -14140,7 +14140,7 @@
       </c>
       <c r="J206" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K206" t="inlineStr">
@@ -14202,12 +14202,12 @@
       </c>
       <c r="I207" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J207" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K207" t="inlineStr">
@@ -14274,7 +14274,7 @@
       </c>
       <c r="J208" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K208" t="inlineStr">
@@ -14341,7 +14341,7 @@
       </c>
       <c r="J209" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K209" t="inlineStr">
@@ -14475,7 +14475,7 @@
       </c>
       <c r="J211" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K211" t="inlineStr">
@@ -18418,7 +18418,7 @@
       </c>
       <c r="H270" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="I270" t="inlineStr">
@@ -21778,7 +21778,7 @@
       </c>
       <c r="J320" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K320" t="inlineStr">
@@ -21845,7 +21845,7 @@
       </c>
       <c r="J321" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K321" t="inlineStr">
@@ -22314,7 +22314,7 @@
       </c>
       <c r="J328" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K328" t="inlineStr">
@@ -22448,7 +22448,7 @@
       </c>
       <c r="J330" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K330" t="inlineStr">
@@ -22515,7 +22515,7 @@
       </c>
       <c r="J331" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K331" t="inlineStr">
@@ -22716,7 +22716,7 @@
       </c>
       <c r="J334" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K334" t="inlineStr">
@@ -22783,7 +22783,7 @@
       </c>
       <c r="J335" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K335" t="inlineStr">
@@ -22850,7 +22850,7 @@
       </c>
       <c r="J336" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K336" t="inlineStr">
@@ -22917,7 +22917,7 @@
       </c>
       <c r="J337" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K337" t="inlineStr">
@@ -22984,7 +22984,7 @@
       </c>
       <c r="J338" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K338" t="inlineStr">
@@ -23051,7 +23051,7 @@
       </c>
       <c r="J339" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K339" t="inlineStr">
@@ -23185,7 +23185,7 @@
       </c>
       <c r="J341" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K341" t="inlineStr">
@@ -23252,7 +23252,7 @@
       </c>
       <c r="J342" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K342" t="inlineStr">
@@ -23654,7 +23654,7 @@
       </c>
       <c r="J348" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K348" t="inlineStr">
@@ -23721,7 +23721,7 @@
       </c>
       <c r="J349" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K349" t="inlineStr">
@@ -23922,7 +23922,7 @@
       </c>
       <c r="J352" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K352" t="inlineStr">
@@ -24123,7 +24123,7 @@
       </c>
       <c r="J355" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K355" t="inlineStr">
@@ -24257,7 +24257,7 @@
       </c>
       <c r="J357" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K357" t="inlineStr">
@@ -24458,7 +24458,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K360" t="inlineStr">
@@ -24659,7 +24659,7 @@
       </c>
       <c r="J363" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K363" t="inlineStr">
@@ -24860,7 +24860,7 @@
       </c>
       <c r="J366" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K366" t="inlineStr">
@@ -25128,7 +25128,7 @@
       </c>
       <c r="J370" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K370" t="inlineStr">
@@ -25262,7 +25262,7 @@
       </c>
       <c r="J372" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K372" t="inlineStr">
@@ -25798,7 +25798,7 @@
       </c>
       <c r="J380" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K380" t="inlineStr">
@@ -25865,7 +25865,7 @@
       </c>
       <c r="J381" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K381" t="inlineStr">
@@ -25999,7 +25999,7 @@
       </c>
       <c r="J383" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K383" t="inlineStr">
@@ -26066,7 +26066,7 @@
       </c>
       <c r="J384" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K384" t="inlineStr">
@@ -26200,7 +26200,7 @@
       </c>
       <c r="J386" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K386" t="inlineStr">
@@ -26937,7 +26937,7 @@
       </c>
       <c r="J397" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K397" t="inlineStr">
@@ -27071,7 +27071,7 @@
       </c>
       <c r="J399" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K399" t="inlineStr">
@@ -27942,7 +27942,7 @@
       </c>
       <c r="J412" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K412" t="inlineStr">
@@ -28277,7 +28277,7 @@
       </c>
       <c r="J417" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K417" t="inlineStr">
@@ -28746,7 +28746,7 @@
       </c>
       <c r="J424" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K424" t="inlineStr">
@@ -29014,7 +29014,7 @@
       </c>
       <c r="J428" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K428" t="inlineStr">
@@ -29148,7 +29148,7 @@
       </c>
       <c r="J430" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K430" t="inlineStr">
@@ -29483,7 +29483,7 @@
       </c>
       <c r="J435" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K435" t="inlineStr">
@@ -29550,7 +29550,7 @@
       </c>
       <c r="J436" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K436" t="inlineStr">
@@ -29684,7 +29684,7 @@
       </c>
       <c r="J438" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K438" t="inlineStr">
@@ -30019,7 +30019,7 @@
       </c>
       <c r="J443" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K443" t="inlineStr">
@@ -30153,7 +30153,7 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -30220,7 +30220,7 @@
       </c>
       <c r="J446" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K446" t="inlineStr">
@@ -30488,7 +30488,7 @@
       </c>
       <c r="J450" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K450" t="inlineStr">
@@ -30555,7 +30555,7 @@
       </c>
       <c r="J451" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K451" t="inlineStr">
@@ -30689,7 +30689,7 @@
       </c>
       <c r="J453" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K453" t="inlineStr">
@@ -30756,7 +30756,7 @@
       </c>
       <c r="J454" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K454" t="inlineStr">
@@ -30823,7 +30823,7 @@
       </c>
       <c r="J455" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K455" t="inlineStr">
@@ -31091,7 +31091,7 @@
       </c>
       <c r="J459" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K459" t="inlineStr">
@@ -31158,7 +31158,7 @@
       </c>
       <c r="J460" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K460" t="inlineStr">
@@ -31359,7 +31359,7 @@
       </c>
       <c r="J463" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K463" t="inlineStr">
@@ -31426,7 +31426,7 @@
       </c>
       <c r="J464" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K464" t="inlineStr">
@@ -31493,7 +31493,7 @@
       </c>
       <c r="J465" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K465" t="inlineStr">
@@ -31694,7 +31694,7 @@
       </c>
       <c r="J468" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K468" t="inlineStr">
@@ -31761,7 +31761,7 @@
       </c>
       <c r="J469" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K469" t="inlineStr">
@@ -31895,7 +31895,7 @@
       </c>
       <c r="J471" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K471" t="inlineStr">
@@ -31962,7 +31962,7 @@
       </c>
       <c r="J472" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K472" t="inlineStr">
@@ -32029,7 +32029,7 @@
       </c>
       <c r="J473" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K473" t="inlineStr">
@@ -32297,7 +32297,7 @@
       </c>
       <c r="J477" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K477" t="inlineStr">
@@ -32431,7 +32431,7 @@
       </c>
       <c r="J479" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K479" t="inlineStr">
@@ -32498,7 +32498,7 @@
       </c>
       <c r="J480" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K480" t="inlineStr">
@@ -32699,7 +32699,7 @@
       </c>
       <c r="J483" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K483" t="inlineStr">
@@ -32766,7 +32766,7 @@
       </c>
       <c r="J484" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K484" t="inlineStr">
@@ -32833,7 +32833,7 @@
       </c>
       <c r="J485" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K485" t="inlineStr">
@@ -32900,7 +32900,7 @@
       </c>
       <c r="J486" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K486" t="inlineStr">
@@ -32967,7 +32967,7 @@
       </c>
       <c r="J487" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K487" t="inlineStr">
@@ -33034,7 +33034,7 @@
       </c>
       <c r="J488" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K488" t="inlineStr">
@@ -33101,7 +33101,7 @@
       </c>
       <c r="J489" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K489" t="inlineStr">
@@ -33168,7 +33168,7 @@
       </c>
       <c r="J490" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K490" t="inlineStr">
@@ -33302,7 +33302,7 @@
       </c>
       <c r="J492" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K492" t="inlineStr">
@@ -33369,7 +33369,7 @@
       </c>
       <c r="J493" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K493" t="inlineStr">
@@ -33436,7 +33436,7 @@
       </c>
       <c r="J494" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K494" t="inlineStr">
@@ -33503,7 +33503,7 @@
       </c>
       <c r="J495" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K495" t="inlineStr">
@@ -33570,7 +33570,7 @@
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
@@ -33637,7 +33637,7 @@
       </c>
       <c r="J497" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K497" t="inlineStr">
@@ -33704,7 +33704,7 @@
       </c>
       <c r="J498" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K498" t="inlineStr">
@@ -33771,7 +33771,7 @@
       </c>
       <c r="J499" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K499" t="inlineStr">
@@ -33838,7 +33838,7 @@
       </c>
       <c r="J500" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K500" t="inlineStr">
@@ -33972,7 +33972,7 @@
       </c>
       <c r="J502" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K502" t="inlineStr">
@@ -34039,7 +34039,7 @@
       </c>
       <c r="J503" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K503" t="inlineStr">
@@ -34106,7 +34106,7 @@
       </c>
       <c r="J504" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K504" t="inlineStr">
@@ -34374,7 +34374,7 @@
       </c>
       <c r="J508" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K508" t="inlineStr">
@@ -34441,7 +34441,7 @@
       </c>
       <c r="J509" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K509" t="inlineStr">
@@ -34508,7 +34508,7 @@
       </c>
       <c r="J510" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K510" t="inlineStr">
@@ -34575,7 +34575,7 @@
       </c>
       <c r="J511" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K511" t="inlineStr">
@@ -34709,7 +34709,7 @@
       </c>
       <c r="J513" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K513" t="inlineStr">
@@ -34776,7 +34776,7 @@
       </c>
       <c r="J514" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K514" t="inlineStr">
@@ -34843,7 +34843,7 @@
       </c>
       <c r="J515" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K515" t="inlineStr">
@@ -34910,7 +34910,7 @@
       </c>
       <c r="J516" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K516" t="inlineStr">
@@ -35245,7 +35245,7 @@
       </c>
       <c r="J521" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K521" t="inlineStr">
@@ -35312,7 +35312,7 @@
       </c>
       <c r="J522" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K522" t="inlineStr">
@@ -35513,7 +35513,7 @@
       </c>
       <c r="J525" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K525" t="inlineStr">
@@ -35647,7 +35647,7 @@
       </c>
       <c r="J527" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K527" t="inlineStr">
@@ -35915,7 +35915,7 @@
       </c>
       <c r="J531" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K531" t="inlineStr">
@@ -36049,7 +36049,7 @@
       </c>
       <c r="J533" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K533" t="inlineStr">
@@ -36183,7 +36183,7 @@
       </c>
       <c r="J535" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K535" t="inlineStr">
@@ -36250,7 +36250,7 @@
       </c>
       <c r="J536" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K536" t="inlineStr">
@@ -36518,7 +36518,7 @@
       </c>
       <c r="J540" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K540" t="inlineStr">
@@ -36585,7 +36585,7 @@
       </c>
       <c r="J541" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K541" t="inlineStr">
@@ -36652,7 +36652,7 @@
       </c>
       <c r="J542" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K542" t="inlineStr">
@@ -36719,7 +36719,7 @@
       </c>
       <c r="J543" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K543" t="inlineStr">
@@ -36853,7 +36853,7 @@
       </c>
       <c r="J545" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K545" t="inlineStr">
@@ -36920,7 +36920,7 @@
       </c>
       <c r="J546" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K546" t="inlineStr">
@@ -36987,7 +36987,7 @@
       </c>
       <c r="J547" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K547" t="inlineStr">
@@ -37054,7 +37054,7 @@
       </c>
       <c r="J548" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K548" t="inlineStr">
@@ -37188,7 +37188,7 @@
       </c>
       <c r="J550" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K550" t="inlineStr">
@@ -37255,7 +37255,7 @@
       </c>
       <c r="J551" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K551" t="inlineStr">
@@ -37322,7 +37322,7 @@
       </c>
       <c r="J552" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K552" t="inlineStr">
@@ -37456,7 +37456,7 @@
       </c>
       <c r="J554" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K554" t="inlineStr">
@@ -37523,7 +37523,7 @@
       </c>
       <c r="J555" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K555" t="inlineStr">
@@ -37590,7 +37590,7 @@
       </c>
       <c r="J556" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K556" t="inlineStr">
@@ -37657,7 +37657,7 @@
       </c>
       <c r="J557" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K557" t="inlineStr">
@@ -37791,7 +37791,7 @@
       </c>
       <c r="J559" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K559" t="inlineStr">
@@ -37858,7 +37858,7 @@
       </c>
       <c r="J560" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K560" t="inlineStr">
@@ -38059,7 +38059,7 @@
       </c>
       <c r="J563" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K563" t="inlineStr">
@@ -38126,7 +38126,7 @@
       </c>
       <c r="J564" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K564" t="inlineStr">
@@ -38327,7 +38327,7 @@
       </c>
       <c r="J567" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K567" t="inlineStr">
@@ -38528,7 +38528,7 @@
       </c>
       <c r="J570" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K570" t="inlineStr">
@@ -38595,7 +38595,7 @@
       </c>
       <c r="J571" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K571" t="inlineStr">
@@ -39198,7 +39198,7 @@
       </c>
       <c r="J580" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K580" t="inlineStr">
@@ -39265,7 +39265,7 @@
       </c>
       <c r="J581" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K581" t="inlineStr">
@@ -39466,7 +39466,7 @@
       </c>
       <c r="J584" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K584" t="inlineStr">
@@ -39533,7 +39533,7 @@
       </c>
       <c r="J585" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K585" t="inlineStr">
@@ -39734,7 +39734,7 @@
       </c>
       <c r="J588" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K588" t="inlineStr">
@@ -39801,7 +39801,7 @@
       </c>
       <c r="J589" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K589" t="inlineStr">
@@ -39935,7 +39935,7 @@
       </c>
       <c r="J591" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K591" t="inlineStr">
@@ -40672,7 +40672,7 @@
       </c>
       <c r="J602" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K602" t="inlineStr">
@@ -40739,7 +40739,7 @@
       </c>
       <c r="J603" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K603" t="inlineStr">
@@ -40806,7 +40806,7 @@
       </c>
       <c r="J604" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K604" t="inlineStr">
@@ -40873,7 +40873,7 @@
       </c>
       <c r="J605" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K605" t="inlineStr">
@@ -41007,7 +41007,7 @@
       </c>
       <c r="J607" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K607" t="inlineStr">
@@ -41074,7 +41074,7 @@
       </c>
       <c r="J608" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K608" t="inlineStr">
@@ -41141,7 +41141,7 @@
       </c>
       <c r="J609" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K609" t="inlineStr">
@@ -41208,7 +41208,7 @@
       </c>
       <c r="J610" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K610" t="inlineStr">
@@ -41275,7 +41275,7 @@
       </c>
       <c r="J611" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K611" t="inlineStr">
@@ -41409,7 +41409,7 @@
       </c>
       <c r="J613" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K613" t="inlineStr">
@@ -41543,7 +41543,7 @@
       </c>
       <c r="J615" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K615" t="inlineStr">
@@ -41610,7 +41610,7 @@
       </c>
       <c r="J616" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K616" t="inlineStr">
@@ -41945,7 +41945,7 @@
       </c>
       <c r="J621" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K621" t="inlineStr">
@@ -42012,7 +42012,7 @@
       </c>
       <c r="J622" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K622" t="inlineStr">
@@ -42213,7 +42213,7 @@
       </c>
       <c r="J625" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K625" t="inlineStr">
@@ -42548,7 +42548,7 @@
       </c>
       <c r="J630" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K630" t="inlineStr">
@@ -42682,7 +42682,7 @@
       </c>
       <c r="J632" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K632" t="inlineStr">
@@ -42749,7 +42749,7 @@
       </c>
       <c r="J633" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K633" t="inlineStr">
@@ -42816,7 +42816,7 @@
       </c>
       <c r="J634" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K634" t="inlineStr">
@@ -42883,7 +42883,7 @@
       </c>
       <c r="J635" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K635" t="inlineStr">
@@ -42950,7 +42950,7 @@
       </c>
       <c r="J636" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K636" t="inlineStr">
@@ -43017,7 +43017,7 @@
       </c>
       <c r="J637" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K637" t="inlineStr">
@@ -43151,7 +43151,7 @@
       </c>
       <c r="J639" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K639" t="inlineStr">
@@ -43419,7 +43419,7 @@
       </c>
       <c r="J643" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K643" t="inlineStr">
@@ -43888,7 +43888,7 @@
       </c>
       <c r="J650" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K650" t="inlineStr">
@@ -43955,7 +43955,7 @@
       </c>
       <c r="J651" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K651" t="inlineStr">
@@ -44960,7 +44960,7 @@
       </c>
       <c r="J666" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K666" t="inlineStr">
@@ -45764,7 +45764,7 @@
       </c>
       <c r="J678" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K678" t="inlineStr">
@@ -45831,7 +45831,7 @@
       </c>
       <c r="J679" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K679" t="inlineStr">
@@ -45898,7 +45898,7 @@
       </c>
       <c r="J680" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K680" t="inlineStr">
@@ -46166,7 +46166,7 @@
       </c>
       <c r="J684" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K684" t="inlineStr">
@@ -46233,7 +46233,7 @@
       </c>
       <c r="J685" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K685" t="inlineStr">
@@ -46367,7 +46367,7 @@
       </c>
       <c r="J687" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K687" t="inlineStr">
@@ -46434,7 +46434,7 @@
       </c>
       <c r="J688" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K688" t="inlineStr">
@@ -46501,7 +46501,7 @@
       </c>
       <c r="J689" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K689" t="inlineStr">
@@ -46568,7 +46568,7 @@
       </c>
       <c r="J690" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K690" t="inlineStr">
@@ -46836,7 +46836,7 @@
       </c>
       <c r="J694" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K694" t="inlineStr">
@@ -46903,7 +46903,7 @@
       </c>
       <c r="J695" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K695" t="inlineStr">
@@ -47037,7 +47037,7 @@
       </c>
       <c r="J697" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K697" t="inlineStr">
@@ -47104,7 +47104,7 @@
       </c>
       <c r="J698" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K698" t="inlineStr">
@@ -47171,7 +47171,7 @@
       </c>
       <c r="J699" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K699" t="inlineStr">
@@ -47640,7 +47640,7 @@
       </c>
       <c r="J706" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K706" t="inlineStr">
@@ -47774,7 +47774,7 @@
       </c>
       <c r="J708" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K708" t="inlineStr">
@@ -48042,7 +48042,7 @@
       </c>
       <c r="J712" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K712" t="inlineStr">
@@ -48980,7 +48980,7 @@
       </c>
       <c r="J726" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K726" t="inlineStr">
@@ -49047,7 +49047,7 @@
       </c>
       <c r="J727" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K727" t="inlineStr">
@@ -49181,7 +49181,7 @@
       </c>
       <c r="J729" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K729" t="inlineStr">
@@ -49248,7 +49248,7 @@
       </c>
       <c r="J730" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K730" t="inlineStr">
@@ -49382,7 +49382,7 @@
       </c>
       <c r="J732" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K732" t="inlineStr">
@@ -49449,7 +49449,7 @@
       </c>
       <c r="J733" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K733" t="inlineStr">
@@ -50119,7 +50119,7 @@
       </c>
       <c r="J743" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K743" t="inlineStr">
@@ -50521,7 +50521,7 @@
       </c>
       <c r="J749" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K749" t="inlineStr">
@@ -50588,7 +50588,7 @@
       </c>
       <c r="J750" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K750" t="inlineStr">
@@ -51459,7 +51459,7 @@
       </c>
       <c r="J763" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K763" t="inlineStr">
@@ -51593,7 +51593,7 @@
       </c>
       <c r="J765" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K765" t="inlineStr">
@@ -53737,7 +53737,7 @@
       </c>
       <c r="J797" t="inlineStr">
         <is>
-          <t>SIM</t>
+          <t>NAO</t>
         </is>
       </c>
       <c r="K797" t="inlineStr">
@@ -58824,12 +58824,12 @@
       </c>
       <c r="I873" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J873" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K873" t="inlineStr">
@@ -59030,7 +59030,7 @@
       </c>
       <c r="J876" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K876" t="inlineStr">
@@ -59097,7 +59097,7 @@
       </c>
       <c r="J877" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K877" t="inlineStr">
@@ -59231,7 +59231,7 @@
       </c>
       <c r="J879" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K879" t="inlineStr">
@@ -59298,7 +59298,7 @@
       </c>
       <c r="J880" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K880" t="inlineStr">
@@ -59628,12 +59628,12 @@
       </c>
       <c r="I885" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="J885" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K885" t="inlineStr">
@@ -59700,7 +59700,7 @@
       </c>
       <c r="J886" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K886" t="inlineStr">
@@ -62447,7 +62447,7 @@
       </c>
       <c r="J927" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K927" t="inlineStr">
@@ -62514,7 +62514,7 @@
       </c>
       <c r="J928" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K928" t="inlineStr">
@@ -62581,7 +62581,7 @@
       </c>
       <c r="J929" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K929" t="inlineStr">
@@ -62648,7 +62648,7 @@
       </c>
       <c r="J930" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K930" t="inlineStr">
@@ -63854,7 +63854,7 @@
       </c>
       <c r="J948" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K948" t="inlineStr">
@@ -63921,7 +63921,7 @@
       </c>
       <c r="J949" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K949" t="inlineStr">
@@ -64055,7 +64055,7 @@
       </c>
       <c r="J951" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K951" t="inlineStr">
@@ -64323,7 +64323,7 @@
       </c>
       <c r="J955" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K955" t="inlineStr">
@@ -64390,7 +64390,7 @@
       </c>
       <c r="J956" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K956" t="inlineStr">
@@ -65127,7 +65127,7 @@
       </c>
       <c r="J967" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K967" t="inlineStr">
@@ -66668,7 +66668,7 @@
       </c>
       <c r="J990" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K990" t="inlineStr">
@@ -66802,7 +66802,7 @@
       </c>
       <c r="J992" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K992" t="inlineStr">
@@ -67070,7 +67070,7 @@
       </c>
       <c r="J996" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K996" t="inlineStr">
@@ -67137,7 +67137,7 @@
       </c>
       <c r="J997" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K997" t="inlineStr">
@@ -67338,7 +67338,7 @@
       </c>
       <c r="J1000" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K1000" t="inlineStr">
@@ -67606,7 +67606,7 @@
       </c>
       <c r="J1004" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K1004" t="inlineStr">
@@ -67673,7 +67673,7 @@
       </c>
       <c r="J1005" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K1005" t="inlineStr">
@@ -67807,7 +67807,7 @@
       </c>
       <c r="J1007" t="inlineStr">
         <is>
-          <t>NAO</t>
+          <t>SIM</t>
         </is>
       </c>
       <c r="K1007" t="inlineStr">

</xml_diff>